<commit_message>
latest changes for login, register and Home page features
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/TestData.xlsx
+++ b/src/test/resources/Excel/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lavanya Yelakala\eclipse-workspace\DSAlgo_TeamAchievers\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E72AEF-2A0F-48A5-88DA-F60FF5BD0C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E70E528-39AA-4FB4-AD1C-3A646E429F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{26669724-F08E-441E-A6A1-80AC505F734B}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="register" sheetId="2" r:id="rId1"/>
     <sheet name="login1" sheetId="3" r:id="rId2"/>
     <sheet name="login" sheetId="5" r:id="rId3"/>
-    <sheet name="pythonCode" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
+    <sheet name="pythonCode" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="85">
   <si>
     <t>username</t>
   </si>
@@ -263,26 +264,86 @@
     <t>Verify that user receives error message for all empty fields during Login</t>
   </si>
   <si>
+    <t>errorMsg</t>
+  </si>
+  <si>
+    <t>Please fill out this field.</t>
+  </si>
+  <si>
+    <t>Password12</t>
+  </si>
+  <si>
     <t>Verify that user receives error message for empty Username field during Login</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>Password12</t>
-  </si>
-  <si>
-    <t>User12345</t>
+    <t>Username25</t>
+  </si>
+  <si>
+    <t>User25677</t>
+  </si>
+  <si>
+    <t>Password6878</t>
+  </si>
+  <si>
+    <t>teamachievers1</t>
+  </si>
+  <si>
+    <t>Password66982</t>
+  </si>
+  <si>
+    <t>Welcome@1234</t>
+  </si>
+  <si>
+    <t>USer9999569</t>
   </si>
   <si>
     <t>Verify that user receives error message for empty Password field during Login</t>
+  </si>
+  <si>
+    <t>Verify that user receives error message for invalid Username and invalid Password fields during Login</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Verify that user receives error message for invalid Username field during Login</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Verify that user receives error message for invalid Password field during Login</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Verify that user able to land on Home page after entering valid Username and Password fields</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>User566677</t>
+  </si>
+  <si>
+    <t>Passwrd787889</t>
+  </si>
+  <si>
+    <t>usertuuhh</t>
+  </si>
+  <si>
+    <t>Psssuejjj</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,6 +386,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -359,7 +426,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -383,6 +450,8 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,7 +790,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -729,7 +798,7 @@
     <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="28.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="1"/>
+    <col min="4" max="4" width="33.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="48.5546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="27.33203125" style="1" customWidth="1"/>
   </cols>
@@ -744,7 +813,9 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
@@ -753,6 +824,9 @@
       </c>
     </row>
     <row r="2" spans="1:6">
+      <c r="D2" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="E2" s="12" t="s">
         <v>4</v>
       </c>
@@ -1000,17 +1074,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DF4F130-7460-44A6-A612-2786A37CAEED}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="63.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1041,21 +1115,149 @@
         <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351C18B5-3A3C-4F9E-AE6C-5DBDCA23E4ED}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1063,7 +1265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C1BB72-E077-4E53-9B8E-2362A02F5343}">
   <dimension ref="A1:B9"/>
   <sheetViews>

</xml_diff>